<commit_message>
[UPDATE] Included fruit waste analysis
</commit_message>
<xml_diff>
--- a/data/food_density_data.xlsx
+++ b/data/food_density_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucapikc_ucl_ac_uk/Documents/Industry/Wynn/Project/FLW/Code/Food_detection/yolov5-fastapi/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive - University College London\Industry\Wynn\Project\FLW\Code\Food_detection\yolov5-fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="14_{7B91F1A8-D48F-4F02-A45E-A2CFDCF37B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD76827F-711C-4E29-95C1-5AB0218768F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3DB39-6849-4B68-BE31-AA88CBBA8229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4D8500EA-26DB-44AB-A7A1-31DA09238ED1}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>Thickness (cm)</t>
   </si>
   <si>
-    <t>168202;	 Apples, raw, golden delicious, with skin; 1 cup is 236.588ml; 1 cup of water is 236.588g (4 degrees C); source from http://foodinfo.us/Densities.aspx; Assume core thickness is 2 cm</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.33 – 0.64 g/cm3 (Yunus2020-INVESTIGATION OF ABSORBENT, ANTIOXIDANT AND THICKENING
 AGENT PROPERTIES OF TROPICAL FRUIT PEELS) take average; 168202; Apples, raw, golden delicious, with skin; source from http://foodinfo.us/Densities.aspx; Assume thickness is 0.5mm</t>
   </si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>Aerssens1998-Interspecies Differences in Bone Composition, Density, and Quality: Potential Implications for in Vivo Bone Research. https://academic.oup.com/endo/article/139/2/663/2987138?login=false; Bone composition: https://www.doitpoms.ac.uk/tlplib/bones/structure.php#:~:text=Bone%20itself%20consists%20mainly%20of,%2D70%25%20is%20bone%20mineral.; Assume 1cm thickenss</t>
+  </si>
+  <si>
+    <t>https://files.eric.ed.gov/fulltext/EJ1107681.pdf found 0.96g/cm3;168202;	 Apples, raw, golden delicious, with skin; 1 cup is 236.588ml; 1 cup of water is 236.588g (4 degrees C); source from http://foodinfo.us/Densities.aspx; Assume core thickness is 2 cm</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,13 +546,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>0.90900000000000003</v>
+        <v>0.96</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -567,7 +567,7 @@
         <v>0.05</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,7 +595,7 @@
         <v>0.3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -639,7 +639,7 @@
         <v>1.25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>0.05</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>